<commit_message>
coordinadores terminado, completo para la presentacion, solo faltan los reportes
</commit_message>
<xml_diff>
--- a/DominicanaLimpia/Pantillas/6.PLANTILLA METAS PARA APLICACION-docentes y personal admon.xlsx
+++ b/DominicanaLimpia/Pantillas/6.PLANTILLA METAS PARA APLICACION-docentes y personal admon.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\Desktop\1.DOMINICANA LIMPIA\4.DOMINICANA LIMPIA-jun2019-dic2019\Presupuestos\5. SISTEMATIZACIÓN\DATOS PARA WILLIAMS\NUEVAS PLANTILLAS COMPLEMENTARIAS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E45E6A-BD92-4E4A-832C-DE4649EB0AAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F8857467-BC64-4908-B2DB-964E45481E44}"/>
   </bookViews>
   <sheets>
     <sheet name="6.DOCENTES Y PERSONAL ADMON" sheetId="1" r:id="rId1"/>
@@ -66,7 +72,7 @@
     <definedName name="_8.Encuentro_en_cada_municipio_con_medios_de_comunicación_e_inicio_Campaña_publicitaria._Anuncio_fecha_de_inicio_recogida_separada_de_los_residuos.">[4]Nombres!$C$16</definedName>
     <definedName name="_9.Compra_de_Equipamiento_y_Puntos_Limpios." localSheetId="0">#REF!</definedName>
     <definedName name="_9.Compra_de_Equipamiento_y_Puntos_Limpios.">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'6.DOCENTES Y PERSONAL ADMON'!$A$1:$E$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'6.DOCENTES Y PERSONAL ADMON'!$A$1:$AB$43</definedName>
     <definedName name="Diseño_e_Impresión_de_documento_instructivo__del_proyecto." localSheetId="0">#REF!</definedName>
     <definedName name="Diseño_e_Impresión_de_documento_instructivo__del_proyecto.">#REF!</definedName>
   </definedNames>
@@ -86,26 +92,17 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={D6504100-CD1D-474C-8309-B19B6E5FA869}</author>
+    <author>tc={29EDE285-2528-4D19-B3BE-3903C32643F3}</author>
   </authors>
   <commentList>
-    <comment ref="F5" authorId="0">
+    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{29EDE285-2528-4D19-B3BE-3903C32643F3}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentario encadenado]
+        <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     Aqui se ingresan los resultados</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -115,16 +112,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
-    <t>METAS  DOCENTES Y PERSONAL ADMINISTRATIVO</t>
-  </si>
-  <si>
-    <t>MUNICIPIOS</t>
-  </si>
-  <si>
     <t xml:space="preserve">POBLACIÓN </t>
-  </si>
-  <si>
-    <t>METAS ESCUELAS -Segundo Semestre 2019</t>
   </si>
   <si>
     <t>Resultado Periodo</t>
@@ -273,14 +261,23 @@
   <si>
     <t>Avance</t>
   </si>
+  <si>
+    <t>METAS PERSONAL ADMINISTRATIVO</t>
+  </si>
+  <si>
+    <t>METAS PERSONAL ADMON -Segundo Semestre 2019</t>
+  </si>
+  <si>
+    <t>TERRITORIO</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -357,14 +354,14 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="16"/>
+      <color theme="0"/>
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -419,8 +416,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -726,15 +729,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
@@ -758,7 +774,7 @@
     <xf numFmtId="3" fontId="5" fillId="8" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
@@ -780,7 +796,7 @@
     <xf numFmtId="3" fontId="5" fillId="8" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -802,7 +818,7 @@
     <xf numFmtId="3" fontId="5" fillId="8" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="8" fillId="9" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -814,26 +830,20 @@
     <xf numFmtId="3" fontId="8" fillId="5" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="8" fillId="5" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="8" fillId="5" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="9" fontId="4" fillId="6" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="6" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -877,14 +887,19 @@
     <xf numFmtId="9" fontId="4" fillId="5" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Millares 2 2" xfId="3"/>
+    <cellStyle name="Millares 2 2" xfId="3" xr:uid="{D64B96B9-061E-4CB5-BBD4-7E218A6D5867}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 4" xfId="2"/>
+    <cellStyle name="Normal 4" xfId="2" xr:uid="{B9D5340F-8FFA-4C32-80B3-782772D1CCFC}"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
-    <cellStyle name="Porcentaje 2" xfId="4"/>
+    <cellStyle name="Porcentaje 2" xfId="4" xr:uid="{3F37B71E-B6AD-4046-AAE4-0BA9E7C173C5}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -900,9 +915,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -944,91 +959,87 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strLit>
-              <c:ptCount val="2"/>
-              <c:pt idx="0">
-                <c:v>#¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF!</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>#¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF!</c:v>
-              </c:pt>
-            </c:strLit>
+            <c:strRef>
+              <c:f>'6.DOCENTES Y PERSONAL ADMON'!$B$7:$B$28</c:f>
+              <c:strCache>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v> AZUA</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v> BANÍ</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v> BÁNICA</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v> CONSTANZA</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v> COTUÍ</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v> DAJABÓN</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>ESPERANZA </c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v> HATO MAYOR</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v> JARABACOA</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v> LOS BOTADOS (D.M.)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v> MAO</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v> MOCA</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v> PUERTO PLATA</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v> SABANA DE LA MAR</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v> SALCEDO</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v> SAN FRANCISCO DE MACORÍS</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v> SAN JOSÉ DE OCOA</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v> SAN JUAN DE LA MAGUANA</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v> SAN PEDRO DE MACORÍS</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v> VERÓN PUNTA CANA (D.M.)</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v> VILLA JARAGUA</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v> VILLA TAPIA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="22"/>
-              <c:pt idx="0">
-                <c:v>59319</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>92153</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>2112</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>34687</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>64133</c:v>
-              </c:pt>
-              <c:pt idx="5">
-                <c:v>25245</c:v>
-              </c:pt>
-              <c:pt idx="6">
-                <c:v>43755</c:v>
-              </c:pt>
-              <c:pt idx="7">
-                <c:v>44900</c:v>
-              </c:pt>
-              <c:pt idx="8">
-                <c:v>40556</c:v>
-              </c:pt>
-              <c:pt idx="9">
-                <c:v>16228</c:v>
-              </c:pt>
-              <c:pt idx="10">
-                <c:v>51647</c:v>
-              </c:pt>
-              <c:pt idx="11">
-                <c:v>94981</c:v>
-              </c:pt>
-              <c:pt idx="12">
-                <c:v>128240</c:v>
-              </c:pt>
-              <c:pt idx="13">
-                <c:v>13723</c:v>
-              </c:pt>
-              <c:pt idx="14">
-                <c:v>35306</c:v>
-              </c:pt>
-              <c:pt idx="15">
-                <c:v>149508</c:v>
-              </c:pt>
-              <c:pt idx="16">
-                <c:v>25710</c:v>
-              </c:pt>
-              <c:pt idx="17">
-                <c:v>78313</c:v>
-              </c:pt>
-              <c:pt idx="18">
-                <c:v>195307</c:v>
-              </c:pt>
-              <c:pt idx="19">
-                <c:v>54128</c:v>
-              </c:pt>
-              <c:pt idx="20">
-                <c:v>10619</c:v>
-              </c:pt>
-              <c:pt idx="21">
-                <c:v>24871</c:v>
-              </c:pt>
-            </c:numLit>
+            <c:numRef>
+              <c:f>'6.DOCENTES Y PERSONAL ADMON'!$C$7:$C$28</c:f>
+            </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-03D1-4E44-AE50-1DBAB6E9DD4D}"/>
+              <c16:uniqueId val="{00000000-4642-4A2D-9A65-C69C76E33434}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1046,91 +1057,87 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strLit>
-              <c:ptCount val="2"/>
-              <c:pt idx="0">
-                <c:v>#¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF!</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>#¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF! #¡REF!</c:v>
-              </c:pt>
-            </c:strLit>
+            <c:strRef>
+              <c:f>'6.DOCENTES Y PERSONAL ADMON'!$B$7:$B$28</c:f>
+              <c:strCache>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v> AZUA</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v> BANÍ</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v> BÁNICA</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v> CONSTANZA</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v> COTUÍ</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v> DAJABÓN</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>ESPERANZA </c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v> HATO MAYOR</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v> JARABACOA</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v> LOS BOTADOS (D.M.)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v> MAO</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v> MOCA</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v> PUERTO PLATA</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v> SABANA DE LA MAR</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v> SALCEDO</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v> SAN FRANCISCO DE MACORÍS</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v> SAN JOSÉ DE OCOA</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v> SAN JUAN DE LA MAGUANA</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v> SAN PEDRO DE MACORÍS</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v> VERÓN PUNTA CANA (D.M.)</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v> VILLA JARAGUA</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v> VILLA TAPIA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="22"/>
-              <c:pt idx="0">
-                <c:v>14829.75</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>23038.25</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>528</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>8671.75</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>16033.25</c:v>
-              </c:pt>
-              <c:pt idx="5">
-                <c:v>6311.25</c:v>
-              </c:pt>
-              <c:pt idx="6">
-                <c:v>10938.75</c:v>
-              </c:pt>
-              <c:pt idx="7">
-                <c:v>11225</c:v>
-              </c:pt>
-              <c:pt idx="8">
-                <c:v>10139</c:v>
-              </c:pt>
-              <c:pt idx="9">
-                <c:v>4057</c:v>
-              </c:pt>
-              <c:pt idx="10">
-                <c:v>12911.75</c:v>
-              </c:pt>
-              <c:pt idx="11">
-                <c:v>23745.25</c:v>
-              </c:pt>
-              <c:pt idx="12">
-                <c:v>32060</c:v>
-              </c:pt>
-              <c:pt idx="13">
-                <c:v>3430.75</c:v>
-              </c:pt>
-              <c:pt idx="14">
-                <c:v>8826.5</c:v>
-              </c:pt>
-              <c:pt idx="15">
-                <c:v>37377</c:v>
-              </c:pt>
-              <c:pt idx="16">
-                <c:v>6427.5</c:v>
-              </c:pt>
-              <c:pt idx="17">
-                <c:v>19578.25</c:v>
-              </c:pt>
-              <c:pt idx="18">
-                <c:v>48826.75</c:v>
-              </c:pt>
-              <c:pt idx="19">
-                <c:v>13532</c:v>
-              </c:pt>
-              <c:pt idx="20">
-                <c:v>2654.75</c:v>
-              </c:pt>
-              <c:pt idx="21">
-                <c:v>6217.75</c:v>
-              </c:pt>
-            </c:numLit>
+            <c:numRef>
+              <c:f>'6.DOCENTES Y PERSONAL ADMON'!$D$7:$D$28</c:f>
+            </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-03D1-4E44-AE50-1DBAB6E9DD4D}"/>
+              <c16:uniqueId val="{00000001-4642-4A2D-9A65-C69C76E33434}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1175,7 +1182,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="es-DO"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -1185,7 +1192,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -1206,148 +1213,78 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>'6.DOCENTES Y PERSONAL ADMON'!$A$7:$B$28</c:f>
-              <c:multiLvlStrCache>
+            <c:strRef>
+              <c:f>'6.DOCENTES Y PERSONAL ADMON'!$B$7:$B$28</c:f>
+              <c:strCache>
                 <c:ptCount val="22"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v> AZUA</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v> BANÍ</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v> BÁNICA</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v> CONSTANZA</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v> COTUÍ</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v> DAJABÓN</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>ESPERANZA </c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v> HATO MAYOR</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v> JARABACOA</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v> LOS BOTADOS (D.M.)</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v> MAO</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v> MOCA</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v> PUERTO PLATA</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v> SABANA DE LA MAR</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v> SALCEDO</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v> SAN FRANCISCO DE MACORÍS</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v> SAN JOSÉ DE OCOA</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v> SAN JUAN DE LA MAGUANA</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v> SAN PEDRO DE MACORÍS</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v> VERÓN PUNTA CANA (D.M.)</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v> VILLA JARAGUA</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v> VILLA TAPIA</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>1</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>2</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>4</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>5</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>6</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>7</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>8</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>9</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>10</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>11</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>12</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>13</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>14</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>15</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>16</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>17</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>18</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>19</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>20</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>21</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>22</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
+                <c:pt idx="0">
+                  <c:v> AZUA</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v> BANÍ</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v> BÁNICA</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v> CONSTANZA</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v> COTUÍ</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v> DAJABÓN</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>ESPERANZA </c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v> HATO MAYOR</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v> JARABACOA</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v> LOS BOTADOS (D.M.)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v> MAO</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v> MOCA</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v> PUERTO PLATA</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v> SABANA DE LA MAR</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v> SALCEDO</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v> SAN FRANCISCO DE MACORÍS</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v> SAN JOSÉ DE OCOA</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v> SAN JUAN DE LA MAGUANA</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v> SAN PEDRO DE MACORÍS</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v> VERÓN PUNTA CANA (D.M.)</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v> VILLA JARAGUA</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v> VILLA TAPIA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1356,77 +1293,77 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>5462</c:v>
+                  <c:v>225</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3462</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>686</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1880</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6039</c:v>
+                  <c:v>334</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2463</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3536</c:v>
+                  <c:v>153</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3418</c:v>
+                  <c:v>134</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3270</c:v>
+                  <c:v>136</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1942</c:v>
+                  <c:v>145</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5609</c:v>
+                  <c:v>224</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3052</c:v>
+                  <c:v>179</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9212</c:v>
+                  <c:v>231</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1453</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2011</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9145</c:v>
+                  <c:v>293</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1965</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>7112</c:v>
+                  <c:v>237</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8940</c:v>
+                  <c:v>161</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2021</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1118</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1288</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-03D1-4E44-AE50-1DBAB6E9DD4D}"/>
+              <c16:uniqueId val="{00000002-4642-4A2D-9A65-C69C76E33434}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1475,7 +1412,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="es-DO"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -1486,7 +1423,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -1507,148 +1444,78 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>'6.DOCENTES Y PERSONAL ADMON'!$A$7:$B$28</c:f>
-              <c:multiLvlStrCache>
+            <c:strRef>
+              <c:f>'6.DOCENTES Y PERSONAL ADMON'!$B$7:$B$28</c:f>
+              <c:strCache>
                 <c:ptCount val="22"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v> AZUA</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v> BANÍ</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v> BÁNICA</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v> CONSTANZA</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v> COTUÍ</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v> DAJABÓN</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>ESPERANZA </c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v> HATO MAYOR</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v> JARABACOA</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v> LOS BOTADOS (D.M.)</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v> MAO</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v> MOCA</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v> PUERTO PLATA</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v> SABANA DE LA MAR</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v> SALCEDO</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v> SAN FRANCISCO DE MACORÍS</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v> SAN JOSÉ DE OCOA</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v> SAN JUAN DE LA MAGUANA</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v> SAN PEDRO DE MACORÍS</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v> VERÓN PUNTA CANA (D.M.)</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v> VILLA JARAGUA</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v> VILLA TAPIA</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>1</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>2</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>4</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>5</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>6</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>7</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>8</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>9</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>10</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>11</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>12</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>13</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>14</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>15</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>16</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>17</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>18</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>19</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>20</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>21</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>22</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
+                <c:pt idx="0">
+                  <c:v> AZUA</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v> BANÍ</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v> BÁNICA</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v> CONSTANZA</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v> COTUÍ</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v> DAJABÓN</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>ESPERANZA </c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v> HATO MAYOR</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v> JARABACOA</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v> LOS BOTADOS (D.M.)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v> MAO</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v> MOCA</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v> PUERTO PLATA</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v> SABANA DE LA MAR</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v> SALCEDO</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v> SAN FRANCISCO DE MACORÍS</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v> SAN JOSÉ DE OCOA</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v> SAN JUAN DE LA MAGUANA</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v> SAN PEDRO DE MACORÍS</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v> VERÓN PUNTA CANA (D.M.)</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v> VILLA JARAGUA</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v> VILLA TAPIA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1657,19 +1524,19 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1000</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>500</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1000</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1725,9 +1592,9 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-03D1-4E44-AE50-1DBAB6E9DD4D}"/>
+              <c16:uniqueId val="{00000003-4642-4A2D-9A65-C69C76E33434}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1741,11 +1608,11 @@
         </c:dLbls>
         <c:gapWidth val="103"/>
         <c:overlap val="100"/>
-        <c:axId val="109475328"/>
-        <c:axId val="109477248"/>
+        <c:axId val="1680088112"/>
+        <c:axId val="1680085936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="109475328"/>
+        <c:axId val="1680088112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1760,37 +1627,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:minorGridlines>
-        <c:title>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1822,10 +1658,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-DO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="109477248"/>
+        <c:crossAx val="1680085936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -1833,17 +1669,17 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109477248"/>
+        <c:axId val="1680085936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109475328"/>
+        <c:crossAx val="1680088112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1880,7 +1716,7 @@
           <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-DO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1888,14 +1724,14 @@
     <c:pageMargins b="0.75" l="0.25" r="0.25" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup orientation="landscape" horizontalDpi="-3"/>
   </c:printSettings>
-  <c:userShapes r:id="rId1"/>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1928,7 +1764,7 @@
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>AVANCES META DOCENTES</a:t>
+              <a:t>AVANCES META</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="es-DO" b="1" baseline="0">
@@ -1936,7 +1772,7 @@
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t> Y PERSONAL ADMINISTRATIVO </a:t>
+              <a:t> PERSONAL ADMINISTRATIVO </a:t>
             </a:r>
             <a:endParaRPr lang="es-DO" b="1">
               <a:solidFill>
@@ -1946,7 +1782,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1955,6 +1790,23 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-DO"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:view3D>
@@ -1962,7 +1814,6 @@
       <c:rotY val="0"/>
       <c:depthPercent val="100"/>
       <c:rAngAx val="0"/>
-      <c:perspective val="30"/>
     </c:view3D>
     <c:floor>
       <c:thickness val="0"/>
@@ -2023,9 +1874,9 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-A564-4D27-9E47-FDD2719D46DD}"/>
+                <c16:uniqueId val="{00000001-3462-4A17-A6C6-D8C1C937227A}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2048,9 +1899,9 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-A564-4D27-9E47-FDD2719D46DD}"/>
+                <c16:uniqueId val="{00000003-3462-4A17-A6C6-D8C1C937227A}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2104,7 +1955,7 @@
               <c:showSerName val="0"/>
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout>
                     <c:manualLayout>
@@ -2116,7 +1967,7 @@
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000001-A564-4D27-9E47-FDD2719D46DD}"/>
+                  <c16:uniqueId val="{00000001-3462-4A17-A6C6-D8C1C937227A}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2181,7 +2032,7 @@
               <c:showSerName val="0"/>
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout>
                     <c:manualLayout>
@@ -2193,7 +2044,7 @@
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-A564-4D27-9E47-FDD2719D46DD}"/>
+                  <c16:uniqueId val="{00000003-3462-4A17-A6C6-D8C1C937227A}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2230,7 +2081,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="es-DO"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -2255,7 +2106,7 @@
                 <a:effectLst/>
               </c:spPr>
             </c:leaderLines>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <a:prstGeom prst="ellipse">
@@ -2290,17 +2141,17 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>85084</c:v>
+                  <c:v>3260</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3501</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-A564-4D27-9E47-FDD2719D46DD}"/>
+              <c16:uniqueId val="{00000004-3462-4A17-A6C6-D8C1C937227A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2324,7 +2175,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2350,20 +2200,20 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-DO"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+    <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2389,7 +2239,7 @@
           <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-DO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3519,7 +3369,7 @@
         <xdr:cNvPr id="2" name="Grupo 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{802BFF27-B404-455A-ADB8-48CD70EB3EC1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C7FCB29-6355-44BA-9A03-AEBC631BF509}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3528,7 +3378,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="8502196" y="179160"/>
-          <a:ext cx="15160625" cy="8561161"/>
+          <a:ext cx="15160625" cy="8672286"/>
           <a:chOff x="4746624" y="158750"/>
           <a:chExt cx="15160625" cy="7381876"/>
         </a:xfrm>
@@ -3538,7 +3388,7 @@
           <xdr:cNvPr id="3" name="Gráfico 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50771C06-7094-4619-A896-69905200EC99}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64D6E96D-DEEC-42E0-B197-A10C142CDA89}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3559,7 +3409,7 @@
           <xdr:cNvPr id="4" name="Grupo 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50C31BA4-18CD-4BB7-81D3-ACD93977360B}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBB94FC4-ABB4-4B06-B970-8A2990746700}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3578,7 +3428,7 @@
             <xdr:cNvPr id="5" name="Grupo 4">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2230006-FC06-4CD0-97A5-B56CE0E284CB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D168BC70-CE44-45BF-BEF0-7AF78424F00C}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3597,7 +3447,7 @@
               <xdr:cNvPr id="9" name="Rectángulo 8">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{422E4190-A045-4C43-B787-E871D0050BB7}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83D755B3-C1A0-43BF-80D8-99BE00CADC92}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -3650,7 +3500,7 @@
               <xdr:cNvPr id="10" name="Rectángulo 9">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{990CAF8C-62EC-4A2B-A3AC-35C8198CF89B}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C1C5800-97ED-485C-A113-E5EA930F9BBC}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -3704,7 +3554,7 @@
             <xdr:cNvPr id="6" name="Grupo 5">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{886EB57F-C171-49F6-97D7-2A8FC09604B5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5899602-15DF-4860-9283-703D00696B6C}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3723,7 +3573,7 @@
               <xdr:cNvPr id="7" name="Rectángulo 6">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9A21A8E-9995-45A8-95FE-4A14E06AE219}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86199F4C-371A-4BD8-A784-36CC57F91C99}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -3776,7 +3626,7 @@
               <xdr:cNvPr id="8" name="Rectángulo 7">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CEEE719-2EC4-44FD-8F9E-A4BA6305E6FE}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{690FF84D-A8F2-4ACD-B303-DA8B4AD47ECA}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -3847,7 +3697,7 @@
         <xdr:cNvPr id="11" name="Globo: flecha hacia abajo 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE9BE5CB-5825-4717-B55F-E61194291BFE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{236AA1F9-6987-480C-809A-A21D4655A381}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3917,7 +3767,7 @@
         <xdr:cNvPr id="12" name="Gráfico 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED11E88E-CB2D-4A28-80AE-BBC576D82FBD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D5F2917-BA92-4CD0-BF6F-0703581FD18F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3944,19 +3794,19 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.0545</cdr:x>
-      <cdr:y>0.03863</cdr:y>
+      <cdr:x>0.21576</cdr:x>
+      <cdr:y>0.05717</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.53903</cdr:x>
-      <cdr:y>0.14701</cdr:y>
+      <cdr:x>0.70029</cdr:x>
+      <cdr:y>0.16714</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
         <cdr:cNvPr id="2" name="Rectángulo 1">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5B98E79-9857-4789-8C16-3C155673B7C8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5B98E79-9857-4789-8C16-3C155673B7C8}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -3964,8 +3814,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="826184" y="335536"/>
-          <a:ext cx="7345778" cy="941377"/>
+          <a:off x="3271013" y="495795"/>
+          <a:ext cx="7345777" cy="953691"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -4002,7 +3852,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </a:rPr>
-            <a:t>METAS DE DOCENTES Y PERSONAL ADMINISTRATIVO</a:t>
+            <a:t>METAS PERSONAL ADMINISTRATIVO</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1800" b="1" cap="none" spc="0" baseline="0">
@@ -4075,7 +3925,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </a:rPr>
-            <a:t> Municipios -</a:t>
+            <a:t> Territorios -</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1800" b="0" cap="none" spc="0">
@@ -4473,7 +4323,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Adriana Mora" id="{CDEAC1C8-6BC1-4B09-8E0E-C63C2147BB3D}" userId="a6827f2dae6e98ff" providerId="Windows Live"/>
+  <person displayName="Adriana Mora" id="{5D334E30-1FA6-4025-B026-321E4E3138A2}" userId="a6827f2dae6e98ff" providerId="Windows Live"/>
 </personList>
 </file>
 
@@ -4520,7 +4370,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -4572,7 +4422,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -4766,7 +4616,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4774,28 +4624,28 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="F5" dT="2019-10-08T14:02:39.17" personId="{CDEAC1C8-6BC1-4B09-8E0E-C63C2147BB3D}" id="{D6504100-CD1D-474C-8309-B19B6E5FA869}">
+  <threadedComment ref="F5" dT="2019-10-08T14:02:39.17" personId="{5D334E30-1FA6-4025-B026-321E4E3138A2}" id="{29EDE285-2528-4D19-B3BE-3903C32643F3}">
     <text>Aqui se ingresan los resultados</text>
   </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C5E9647-CF36-49AC-AFFA-E641532B957F}">
   <sheetPr>
     <tabColor rgb="FF159BFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AJ72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A6" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H13" sqref="H13"/>
+      <selection pane="topRight" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="37" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" style="36" customWidth="1"/>
     <col min="2" max="2" width="42.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" style="3" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" style="3" hidden="1" customWidth="1"/>
@@ -4809,63 +4659,63 @@
       <c r="A1" s="1"/>
     </row>
     <row r="2" spans="1:36" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
+      <c r="A2" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
     </row>
     <row r="3" spans="1:36" s="2" customFormat="1" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="42"/>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
+      <c r="A3" s="40"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
     </row>
     <row r="4" spans="1:36" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="45"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="43"/>
     </row>
     <row r="5" spans="1:36" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="45"/>
+      <c r="C5" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="50">
+        <v>0.25</v>
+      </c>
+      <c r="E5" s="52" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="47"/>
-      <c r="C5" s="50" t="s">
+      <c r="G5" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="52">
-        <v>0.25</v>
-      </c>
-      <c r="E5" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="38" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:36" s="4" customFormat="1" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="48"/>
-      <c r="B6" s="49"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="55"/>
+    </row>
+    <row r="6" spans="1:36" s="4" customFormat="1" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="46"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="53"/>
       <c r="F6" s="39"/>
       <c r="G6" s="39"/>
     </row>
     <row r="7" spans="1:36" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C7" s="7">
         <v>59319</v>
@@ -4875,22 +4725,22 @@
         <v>14829.75</v>
       </c>
       <c r="E7" s="9">
-        <v>5462</v>
+        <v>225</v>
       </c>
       <c r="F7" s="10">
-        <v>1000</v>
+        <v>20</v>
       </c>
       <c r="G7" s="11">
         <f>+F7/E7</f>
-        <v>0.18308311973636029</v>
+        <v>8.8888888888888892E-2</v>
       </c>
     </row>
     <row r="8" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C8" s="15">
         <v>92153</v>
@@ -4900,14 +4750,14 @@
         <v>23038.25</v>
       </c>
       <c r="E8" s="17">
-        <v>3462</v>
+        <v>115</v>
       </c>
       <c r="F8" s="18">
-        <v>1000</v>
+        <v>20</v>
       </c>
       <c r="G8" s="19">
         <f t="shared" ref="G8:G28" si="1">+F8/E8</f>
-        <v>0.28885037550548814</v>
+        <v>0.17391304347826086</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -4941,10 +4791,10 @@
     </row>
     <row r="9" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C9" s="15">
         <v>2112</v>
@@ -4954,14 +4804,14 @@
         <v>528</v>
       </c>
       <c r="E9" s="17">
-        <v>686</v>
+        <v>83</v>
       </c>
       <c r="F9" s="18">
-        <v>500</v>
+        <v>20</v>
       </c>
       <c r="G9" s="19">
         <f t="shared" si="1"/>
-        <v>0.7288629737609329</v>
+        <v>0.24096385542168675</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -4995,10 +4845,10 @@
     </row>
     <row r="10" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C10" s="15">
         <v>34687</v>
@@ -5008,14 +4858,14 @@
         <v>8671.75</v>
       </c>
       <c r="E10" s="17">
-        <v>1880</v>
+        <v>50</v>
       </c>
       <c r="F10" s="18">
-        <v>1000</v>
+        <v>20</v>
       </c>
       <c r="G10" s="19">
         <f t="shared" si="1"/>
-        <v>0.53191489361702127</v>
+        <v>0.4</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -5049,10 +4899,10 @@
     </row>
     <row r="11" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C11" s="15">
         <v>64133</v>
@@ -5062,14 +4912,14 @@
         <v>16033.25</v>
       </c>
       <c r="E11" s="17">
-        <v>6039</v>
+        <v>334</v>
       </c>
       <c r="F11" s="18">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="G11" s="19">
         <f t="shared" si="1"/>
-        <v>1.6559032952475575E-4</v>
+        <v>5.9880239520958084E-2</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -5103,10 +4953,10 @@
     </row>
     <row r="12" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C12" s="15">
         <v>25245</v>
@@ -5116,7 +4966,7 @@
         <v>6311.25</v>
       </c>
       <c r="E12" s="17">
-        <v>2463</v>
+        <v>150</v>
       </c>
       <c r="F12" s="18">
         <v>0</v>
@@ -5157,10 +5007,10 @@
     </row>
     <row r="13" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C13" s="15">
         <v>43755</v>
@@ -5170,7 +5020,7 @@
         <v>10938.75</v>
       </c>
       <c r="E13" s="17">
-        <v>3536</v>
+        <v>153</v>
       </c>
       <c r="F13" s="18">
         <v>0</v>
@@ -5179,7 +5029,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H13" s="56"/>
+      <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -5211,10 +5061,10 @@
     </row>
     <row r="14" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C14" s="15">
         <v>44900</v>
@@ -5224,7 +5074,7 @@
         <v>11225</v>
       </c>
       <c r="E14" s="17">
-        <v>3418</v>
+        <v>134</v>
       </c>
       <c r="F14" s="18">
         <v>0</v>
@@ -5265,10 +5115,10 @@
     </row>
     <row r="15" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C15" s="15">
         <v>40556</v>
@@ -5278,7 +5128,7 @@
         <v>10139</v>
       </c>
       <c r="E15" s="17">
-        <v>3270</v>
+        <v>136</v>
       </c>
       <c r="F15" s="18">
         <v>0</v>
@@ -5319,10 +5169,10 @@
     </row>
     <row r="16" spans="1:36" ht="18" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C16" s="15">
         <v>16228</v>
@@ -5332,7 +5182,7 @@
         <v>4057</v>
       </c>
       <c r="E16" s="17">
-        <v>1942</v>
+        <v>145</v>
       </c>
       <c r="F16" s="18">
         <v>0</v>
@@ -5373,10 +5223,10 @@
     </row>
     <row r="17" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C17" s="15">
         <v>51647</v>
@@ -5386,7 +5236,7 @@
         <v>12911.75</v>
       </c>
       <c r="E17" s="17">
-        <v>5609</v>
+        <v>224</v>
       </c>
       <c r="F17" s="18">
         <v>0</v>
@@ -5427,10 +5277,10 @@
     </row>
     <row r="18" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C18" s="15">
         <v>94981</v>
@@ -5440,7 +5290,7 @@
         <v>23745.25</v>
       </c>
       <c r="E18" s="17">
-        <v>3052</v>
+        <v>179</v>
       </c>
       <c r="F18" s="18">
         <v>0</v>
@@ -5481,10 +5331,10 @@
     </row>
     <row r="19" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C19" s="15">
         <v>128240</v>
@@ -5494,7 +5344,7 @@
         <v>32060</v>
       </c>
       <c r="E19" s="17">
-        <v>9212</v>
+        <v>231</v>
       </c>
       <c r="F19" s="18">
         <v>0</v>
@@ -5535,10 +5385,10 @@
     </row>
     <row r="20" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C20" s="15">
         <v>13723</v>
@@ -5548,7 +5398,7 @@
         <v>3430.75</v>
       </c>
       <c r="E20" s="17">
-        <v>1453</v>
+        <v>60</v>
       </c>
       <c r="F20" s="18">
         <v>0</v>
@@ -5589,10 +5439,10 @@
     </row>
     <row r="21" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C21" s="15">
         <v>35306</v>
@@ -5602,7 +5452,7 @@
         <v>8826.5</v>
       </c>
       <c r="E21" s="17">
-        <v>2011</v>
+        <v>121</v>
       </c>
       <c r="F21" s="18">
         <v>0</v>
@@ -5643,10 +5493,10 @@
     </row>
     <row r="22" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C22" s="15">
         <v>149508</v>
@@ -5656,7 +5506,7 @@
         <v>37377</v>
       </c>
       <c r="E22" s="17">
-        <v>9145</v>
+        <v>293</v>
       </c>
       <c r="F22" s="18">
         <v>0</v>
@@ -5697,10 +5547,10 @@
     </row>
     <row r="23" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C23" s="15">
         <v>25710</v>
@@ -5710,7 +5560,7 @@
         <v>6427.5</v>
       </c>
       <c r="E23" s="17">
-        <v>1965</v>
+        <v>82</v>
       </c>
       <c r="F23" s="18">
         <v>0</v>
@@ -5751,10 +5601,10 @@
     </row>
     <row r="24" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C24" s="15">
         <v>78313</v>
@@ -5764,7 +5614,7 @@
         <v>19578.25</v>
       </c>
       <c r="E24" s="17">
-        <v>7112</v>
+        <v>237</v>
       </c>
       <c r="F24" s="18">
         <v>0</v>
@@ -5805,10 +5655,10 @@
     </row>
     <row r="25" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C25" s="15">
         <v>195307</v>
@@ -5818,7 +5668,7 @@
         <v>48826.75</v>
       </c>
       <c r="E25" s="17">
-        <v>8940</v>
+        <v>161</v>
       </c>
       <c r="F25" s="18">
         <v>0</v>
@@ -5859,10 +5709,10 @@
     </row>
     <row r="26" spans="1:36" ht="18" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C26" s="15">
         <v>54128</v>
@@ -5872,7 +5722,7 @@
         <v>13532</v>
       </c>
       <c r="E26" s="17">
-        <v>2021</v>
+        <v>18</v>
       </c>
       <c r="F26" s="18">
         <v>0</v>
@@ -5913,10 +5763,10 @@
     </row>
     <row r="27" spans="1:36" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C27" s="15">
         <v>10619</v>
@@ -5926,7 +5776,7 @@
         <v>2654.75</v>
       </c>
       <c r="E27" s="17">
-        <v>1118</v>
+        <v>57</v>
       </c>
       <c r="F27" s="18">
         <v>0</v>
@@ -5938,10 +5788,10 @@
     </row>
     <row r="28" spans="1:36" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="21" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C28" s="23">
         <v>24871</v>
@@ -5951,7 +5801,7 @@
         <v>6217.75</v>
       </c>
       <c r="E28" s="25">
-        <v>1288</v>
+        <v>72</v>
       </c>
       <c r="F28" s="26">
         <v>0</v>
@@ -5990,11 +5840,11 @@
       <c r="AI28" s="2"/>
       <c r="AJ28" s="2"/>
     </row>
-    <row r="29" spans="1:36" s="33" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="B29" s="41"/>
+    <row r="29" spans="1:36" s="32" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="55"/>
       <c r="C29" s="28">
         <f>SUM(C7:C28)</f>
         <v>1285441</v>
@@ -6005,50 +5855,50 @@
       </c>
       <c r="E29" s="29">
         <f t="shared" si="2"/>
-        <v>85084</v>
+        <v>3260</v>
       </c>
       <c r="F29" s="30">
         <f>SUM(F7:F28)</f>
-        <v>3501</v>
-      </c>
-      <c r="G29" s="31">
+        <v>100</v>
+      </c>
+      <c r="G29" s="37">
         <f>+F29/E29</f>
-        <v>4.1147571811386396E-2</v>
-      </c>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="32"/>
-      <c r="K29" s="32"/>
-      <c r="L29" s="32"/>
-      <c r="M29" s="32"/>
-      <c r="N29" s="32"/>
-      <c r="O29" s="32"/>
-      <c r="P29" s="32"/>
-      <c r="Q29" s="32"/>
-      <c r="R29" s="32"/>
-      <c r="S29" s="32"/>
-      <c r="T29" s="32"/>
-      <c r="U29" s="32"/>
-      <c r="V29" s="32"/>
-      <c r="W29" s="32"/>
-      <c r="X29" s="32"/>
-      <c r="Y29" s="32"/>
-      <c r="Z29" s="32"/>
-      <c r="AA29" s="32"/>
-      <c r="AB29" s="32"/>
-      <c r="AC29" s="32"/>
-      <c r="AD29" s="32"/>
-      <c r="AE29" s="32"/>
-      <c r="AF29" s="32"/>
-      <c r="AG29" s="32"/>
-      <c r="AH29" s="32"/>
-      <c r="AI29" s="32"/>
-      <c r="AJ29" s="32"/>
+        <v>3.0674846625766871E-2</v>
+      </c>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
+      <c r="K29" s="31"/>
+      <c r="L29" s="31"/>
+      <c r="M29" s="31"/>
+      <c r="N29" s="31"/>
+      <c r="O29" s="31"/>
+      <c r="P29" s="31"/>
+      <c r="Q29" s="31"/>
+      <c r="R29" s="31"/>
+      <c r="S29" s="31"/>
+      <c r="T29" s="31"/>
+      <c r="U29" s="31"/>
+      <c r="V29" s="31"/>
+      <c r="W29" s="31"/>
+      <c r="X29" s="31"/>
+      <c r="Y29" s="31"/>
+      <c r="Z29" s="31"/>
+      <c r="AA29" s="31"/>
+      <c r="AB29" s="31"/>
+      <c r="AC29" s="31"/>
+      <c r="AD29" s="31"/>
+      <c r="AE29" s="31"/>
+      <c r="AF29" s="31"/>
+      <c r="AG29" s="31"/>
+      <c r="AH29" s="31"/>
+      <c r="AI29" s="31"/>
+      <c r="AJ29" s="31"/>
     </row>
     <row r="30" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
     </row>
     <row r="31" spans="1:36" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
@@ -6059,13 +5909,13 @@
     <row r="33" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -6076,11 +5926,11 @@
     </row>
     <row r="37" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
-      <c r="E37" s="35"/>
+      <c r="E37" s="34"/>
     </row>
     <row r="38" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
-      <c r="E38" s="36"/>
+      <c r="E38" s="35"/>
     </row>
     <row r="39" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
@@ -6210,7 +6060,7 @@
   </conditionalFormatting>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="5" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="5" scale="47" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>

</xml_diff>